<commit_message>
Update: example and sticky legend
</commit_message>
<xml_diff>
--- a/file/criterion-template-long.xlsx
+++ b/file/criterion-template-long.xlsx
@@ -1,30 +1,24 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21001"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19126"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Dropbox\Ongoing - Dropbox\app-AHP\ref\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\chihy\Dropbox\Ongoing - Dropbox\app-AHP\file\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F5ADA135-D7DE-4AFA-9A60-48122811FB1A}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{7E24BE01-4D1C-47B6-9635-F57FDC210AF9}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15540" windowHeight="10240" xr2:uid="{37971D20-4150-4350-954F-912B86F59D3D}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15540" windowHeight="10238" xr2:uid="{37971D20-4150-4350-954F-912B86F59D3D}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="179017"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -39,12 +33,6 @@
     <t>Criteria</t>
   </si>
   <si>
-    <t>Accounting firm</t>
-  </si>
-  <si>
-    <t>Consulting firm</t>
-  </si>
-  <si>
     <t>Entry</t>
   </si>
   <si>
@@ -165,12 +153,6 @@
     <t>Present</t>
   </si>
   <si>
-    <t>Banking</t>
-  </si>
-  <si>
-    <t>Tech firm</t>
-  </si>
-  <si>
     <t>Colleague</t>
   </si>
   <si>
@@ -190,6 +172,18 @@
   </si>
   <si>
     <t>Bonus</t>
+  </si>
+  <si>
+    <t>Pear Company</t>
+  </si>
+  <si>
+    <t>Cherry Enterprise</t>
+  </si>
+  <si>
+    <t>Grape Startup</t>
+  </si>
+  <si>
+    <t>Banana Firm</t>
   </si>
 </sst>
 </file>
@@ -545,16 +539,16 @@
   <dimension ref="A1:E36"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F23" sqref="F23"/>
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="15.54296875" customWidth="1"/>
-    <col min="2" max="4" width="16.54296875" customWidth="1"/>
+    <col min="1" max="1" width="15.53125" customWidth="1"/>
+    <col min="2" max="4" width="16.53125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -564,227 +558,227 @@
       <c r="C1" s="1"/>
       <c r="D1" s="1"/>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
+        <v>52</v>
+      </c>
+      <c r="B2" t="s">
         <v>2</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A3" t="s">
+        <v>49</v>
+      </c>
+      <c r="C3" t="s">
         <v>4</v>
       </c>
-      <c r="C2" t="s">
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A4" t="s">
+        <v>50</v>
+      </c>
+      <c r="C4" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A3" t="s">
-        <v>3</v>
-      </c>
-      <c r="C3" t="s">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A5" t="s">
+        <v>51</v>
+      </c>
+      <c r="C5" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A4" t="s">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="B6" t="s">
+        <v>7</v>
+      </c>
+      <c r="C6" t="s">
+        <v>8</v>
+      </c>
+      <c r="D6" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="D7" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="D8" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="C9" t="s">
+        <v>9</v>
+      </c>
+      <c r="D9" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="D10" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="D11" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="C12" t="s">
+        <v>10</v>
+      </c>
+      <c r="D12" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="D13" t="s">
+        <v>33</v>
+      </c>
+      <c r="E13" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="E14" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="E15" t="s">
         <v>44</v>
       </c>
-      <c r="C4" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A5" t="s">
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="D16" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="17" spans="2:5" x14ac:dyDescent="0.45">
+      <c r="C17" t="s">
+        <v>11</v>
+      </c>
+      <c r="D17" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="18" spans="2:5" x14ac:dyDescent="0.45">
+      <c r="D18" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="19" spans="2:5" x14ac:dyDescent="0.45">
+      <c r="D19" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="20" spans="2:5" x14ac:dyDescent="0.45">
+      <c r="D20" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="21" spans="2:5" x14ac:dyDescent="0.45">
+      <c r="C21" t="s">
+        <v>12</v>
+      </c>
+      <c r="D21" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="22" spans="2:5" x14ac:dyDescent="0.45">
+      <c r="D22" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="23" spans="2:5" x14ac:dyDescent="0.45">
+      <c r="D23" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="24" spans="2:5" x14ac:dyDescent="0.45">
+      <c r="D24" t="s">
         <v>45</v>
       </c>
-      <c r="C5" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="B6" t="s">
-        <v>9</v>
-      </c>
-      <c r="C6" t="s">
-        <v>10</v>
-      </c>
-      <c r="D6" t="s">
+      <c r="E24" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="25" spans="2:5" x14ac:dyDescent="0.45">
+      <c r="E25" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="26" spans="2:5" x14ac:dyDescent="0.45">
+      <c r="E26" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="27" spans="2:5" x14ac:dyDescent="0.45">
+      <c r="B27" t="s">
+        <v>13</v>
+      </c>
+      <c r="C27" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="28" spans="2:5" x14ac:dyDescent="0.45">
+      <c r="C28" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="29" spans="2:5" x14ac:dyDescent="0.45">
+      <c r="C29" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="30" spans="2:5" x14ac:dyDescent="0.45">
+      <c r="C30" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="31" spans="2:5" x14ac:dyDescent="0.45">
+      <c r="B31" t="s">
+        <v>17</v>
+      </c>
+      <c r="C31" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="32" spans="2:5" x14ac:dyDescent="0.45">
+      <c r="C32" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="33" spans="3:4" x14ac:dyDescent="0.45">
+      <c r="C33" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="34" spans="3:4" x14ac:dyDescent="0.45">
+      <c r="C34" t="s">
+        <v>21</v>
+      </c>
+      <c r="D34" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="D7" t="s">
+    <row r="35" spans="3:4" x14ac:dyDescent="0.45">
+      <c r="D35" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="D8" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="C9" t="s">
-        <v>11</v>
-      </c>
-      <c r="D9" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="D10" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="D11" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="C12" t="s">
-        <v>12</v>
-      </c>
-      <c r="D12" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="D13" t="s">
-        <v>35</v>
-      </c>
-      <c r="E13" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="E14" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="E15" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="D16" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="17" spans="2:5" x14ac:dyDescent="0.35">
-      <c r="C17" t="s">
-        <v>13</v>
-      </c>
-      <c r="D17" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="18" spans="2:5" x14ac:dyDescent="0.35">
-      <c r="D18" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="19" spans="2:5" x14ac:dyDescent="0.35">
-      <c r="D19" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="20" spans="2:5" x14ac:dyDescent="0.35">
-      <c r="D20" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="21" spans="2:5" x14ac:dyDescent="0.35">
-      <c r="C21" t="s">
-        <v>14</v>
-      </c>
-      <c r="D21" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="22" spans="2:5" x14ac:dyDescent="0.35">
-      <c r="D22" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="23" spans="2:5" x14ac:dyDescent="0.35">
-      <c r="D23" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="24" spans="2:5" x14ac:dyDescent="0.35">
-      <c r="D24" t="s">
-        <v>49</v>
-      </c>
-      <c r="E24" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="25" spans="2:5" x14ac:dyDescent="0.35">
-      <c r="E25" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="26" spans="2:5" x14ac:dyDescent="0.35">
-      <c r="E26" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="27" spans="2:5" x14ac:dyDescent="0.35">
-      <c r="B27" t="s">
-        <v>15</v>
-      </c>
-      <c r="C27" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="28" spans="2:5" x14ac:dyDescent="0.35">
-      <c r="C28" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="29" spans="2:5" x14ac:dyDescent="0.35">
-      <c r="C29" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="30" spans="2:5" x14ac:dyDescent="0.35">
-      <c r="C30" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="31" spans="2:5" x14ac:dyDescent="0.35">
-      <c r="B31" t="s">
-        <v>19</v>
-      </c>
-      <c r="C31" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="32" spans="2:5" x14ac:dyDescent="0.35">
-      <c r="C32" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="33" spans="3:4" x14ac:dyDescent="0.35">
-      <c r="C33" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="34" spans="3:4" x14ac:dyDescent="0.35">
-      <c r="C34" t="s">
-        <v>23</v>
-      </c>
-      <c r="D34" t="s">
+    <row r="36" spans="3:4" x14ac:dyDescent="0.45">
+      <c r="D36" t="s">
         <v>26</v>
-      </c>
-    </row>
-    <row r="35" spans="3:4" x14ac:dyDescent="0.35">
-      <c r="D35" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="36" spans="3:4" x14ac:dyDescent="0.35">
-      <c r="D36" t="s">
-        <v>28</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update: input format and prompt integration
</commit_message>
<xml_diff>
--- a/file/criterion-template-long.xlsx
+++ b/file/criterion-template-long.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\chihy\Dropbox\Ongoing - Dropbox\app-AHP\file\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{FF928979-50A2-43C0-BF59-E952E69DF1E6}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{87DC8B99-98E7-4FC3-8564-4753FD5ED2F8}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="15540" windowHeight="10238" xr2:uid="{37971D20-4150-4350-954F-912B86F59D3D}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="55">
   <si>
     <t>Options</t>
   </si>
@@ -186,13 +186,10 @@
     <t>Banana Firm</t>
   </si>
   <si>
-    <t>Level-1</t>
-  </si>
-  <si>
-    <t>Level-2</t>
-  </si>
-  <si>
-    <t>Level-3</t>
+    <t>Decision</t>
+  </si>
+  <si>
+    <t>Hello World</t>
   </si>
 </sst>
 </file>
@@ -545,260 +542,257 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FA7E53A6-C034-4709-831A-BA74DB0D8F78}">
-  <dimension ref="A1:F37"/>
+  <dimension ref="A1:E38"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="1" max="1" width="15.53125" customWidth="1"/>
-    <col min="2" max="2" width="3" customWidth="1"/>
-    <col min="3" max="5" width="16.53125" customWidth="1"/>
+    <col min="2" max="4" width="16.53125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
+        <v>53</v>
+      </c>
+      <c r="B1" t="s">
+        <v>54</v>
+      </c>
+      <c r="C1" s="1"/>
+      <c r="D1" s="1"/>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A2" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="B2" t="s">
+        <v>52</v>
+      </c>
+      <c r="C2" t="s">
+        <v>49</v>
+      </c>
+      <c r="D2" t="s">
+        <v>50</v>
+      </c>
+      <c r="E2" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="4.5" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A4" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="1"/>
-      <c r="E1" s="1"/>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="C2" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A3" t="s">
-        <v>52</v>
-      </c>
-      <c r="C3" t="s">
+      <c r="B4" t="s">
         <v>2</v>
       </c>
-      <c r="D3" t="s">
+      <c r="C4" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A4" t="s">
-        <v>49</v>
-      </c>
-      <c r="D4" t="s">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="C5" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A5" t="s">
-        <v>50</v>
-      </c>
-      <c r="D5" t="s">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="C6" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A6" t="s">
-        <v>51</v>
-      </c>
-      <c r="D6" t="s">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="C7" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="C7" t="s">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="B8" t="s">
         <v>7</v>
       </c>
-      <c r="D7" t="s">
+      <c r="C8" t="s">
         <v>8</v>
       </c>
-      <c r="E7" t="s">
+      <c r="D8" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="E8" t="s">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="D9" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="E9" t="s">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="D10" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="D10" t="s">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="C11" t="s">
         <v>9</v>
       </c>
-      <c r="E10" t="s">
+      <c r="D11" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="E11" t="s">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="D12" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="E12" t="s">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="D13" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="D13" t="s">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="C14" t="s">
         <v>10</v>
       </c>
-      <c r="E13" t="s">
+      <c r="D14" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="E14" t="s">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="D15" t="s">
         <v>33</v>
       </c>
-      <c r="F14" t="s">
+      <c r="E15" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="F15" t="s">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="E16" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="F16" t="s">
+    <row r="17" spans="2:5" x14ac:dyDescent="0.45">
+      <c r="E17" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="17" spans="3:6" x14ac:dyDescent="0.45">
-      <c r="E17" t="s">
+    <row r="18" spans="2:5" x14ac:dyDescent="0.45">
+      <c r="D18" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="18" spans="3:6" x14ac:dyDescent="0.45">
-      <c r="D18" t="s">
+    <row r="19" spans="2:5" x14ac:dyDescent="0.45">
+      <c r="C19" t="s">
         <v>11</v>
       </c>
-      <c r="E18" t="s">
+      <c r="D19" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="19" spans="3:6" x14ac:dyDescent="0.45">
-      <c r="E19" t="s">
+    <row r="20" spans="2:5" x14ac:dyDescent="0.45">
+      <c r="D20" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="20" spans="3:6" x14ac:dyDescent="0.45">
-      <c r="E20" t="s">
+    <row r="21" spans="2:5" x14ac:dyDescent="0.45">
+      <c r="D21" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="21" spans="3:6" x14ac:dyDescent="0.45">
-      <c r="E21" t="s">
+    <row r="22" spans="2:5" x14ac:dyDescent="0.45">
+      <c r="D22" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="22" spans="3:6" x14ac:dyDescent="0.45">
-      <c r="D22" t="s">
+    <row r="23" spans="2:5" x14ac:dyDescent="0.45">
+      <c r="C23" t="s">
         <v>12</v>
       </c>
-      <c r="E22" t="s">
+      <c r="D23" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="23" spans="3:6" x14ac:dyDescent="0.45">
-      <c r="E23" t="s">
+    <row r="24" spans="2:5" x14ac:dyDescent="0.45">
+      <c r="D24" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="24" spans="3:6" x14ac:dyDescent="0.45">
-      <c r="E24" t="s">
+    <row r="25" spans="2:5" x14ac:dyDescent="0.45">
+      <c r="D25" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="25" spans="3:6" x14ac:dyDescent="0.45">
-      <c r="E25" t="s">
+    <row r="26" spans="2:5" x14ac:dyDescent="0.45">
+      <c r="D26" t="s">
         <v>45</v>
       </c>
-      <c r="F25" t="s">
+      <c r="E26" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="26" spans="3:6" x14ac:dyDescent="0.45">
-      <c r="F26" t="s">
+    <row r="27" spans="2:5" x14ac:dyDescent="0.45">
+      <c r="E27" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="27" spans="3:6" x14ac:dyDescent="0.45">
-      <c r="F27" t="s">
+    <row r="28" spans="2:5" x14ac:dyDescent="0.45">
+      <c r="E28" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="28" spans="3:6" x14ac:dyDescent="0.45">
-      <c r="C28" t="s">
+    <row r="29" spans="2:5" x14ac:dyDescent="0.45">
+      <c r="B29" t="s">
         <v>13</v>
       </c>
-      <c r="D28" t="s">
+      <c r="C29" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="29" spans="3:6" x14ac:dyDescent="0.45">
-      <c r="D29" t="s">
+    <row r="30" spans="2:5" x14ac:dyDescent="0.45">
+      <c r="C30" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="30" spans="3:6" x14ac:dyDescent="0.45">
-      <c r="D30" t="s">
+    <row r="31" spans="2:5" x14ac:dyDescent="0.45">
+      <c r="C31" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="31" spans="3:6" x14ac:dyDescent="0.45">
-      <c r="D31" t="s">
+    <row r="32" spans="2:5" x14ac:dyDescent="0.45">
+      <c r="C32" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="32" spans="3:6" x14ac:dyDescent="0.45">
-      <c r="C32" t="s">
+    <row r="33" spans="2:4" x14ac:dyDescent="0.45">
+      <c r="B33" t="s">
         <v>17</v>
       </c>
-      <c r="D32" t="s">
+      <c r="C33" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="33" spans="4:5" x14ac:dyDescent="0.45">
-      <c r="D33" t="s">
+    <row r="34" spans="2:4" x14ac:dyDescent="0.45">
+      <c r="C34" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="34" spans="4:5" x14ac:dyDescent="0.45">
-      <c r="D34" t="s">
+    <row r="35" spans="2:4" x14ac:dyDescent="0.45">
+      <c r="C35" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="35" spans="4:5" x14ac:dyDescent="0.45">
-      <c r="D35" t="s">
+    <row r="36" spans="2:4" x14ac:dyDescent="0.45">
+      <c r="C36" t="s">
         <v>21</v>
       </c>
-      <c r="E35" t="s">
+      <c r="D36" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="36" spans="4:5" x14ac:dyDescent="0.45">
-      <c r="E36" t="s">
+    <row r="37" spans="2:4" x14ac:dyDescent="0.45">
+      <c r="D37" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="37" spans="4:5" x14ac:dyDescent="0.45">
-      <c r="E37" t="s">
+    <row r="38" spans="2:4" x14ac:dyDescent="0.45">
+      <c r="D38" t="s">
         <v>26</v>
       </c>
     </row>

</xml_diff>